<commit_message>
Add report and update benchmarks.
</commit_message>
<xml_diff>
--- a/docs/Benchmark.xlsx
+++ b/docs/Benchmark.xlsx
@@ -464,11 +464,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1552512815"/>
-        <c:axId val="1010286373"/>
+        <c:axId val="795561413"/>
+        <c:axId val="1254766022"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1552512815"/>
+        <c:axId val="795561413"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -520,10 +520,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1010286373"/>
+        <c:crossAx val="1254766022"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1010286373"/>
+        <c:axId val="1254766022"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -587,7 +587,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1552512815"/>
+        <c:crossAx val="795561413"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -733,11 +733,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1773048964"/>
-        <c:axId val="1498051113"/>
+        <c:axId val="627810477"/>
+        <c:axId val="1221776316"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1773048964"/>
+        <c:axId val="627810477"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -789,10 +789,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1498051113"/>
+        <c:crossAx val="1221776316"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1498051113"/>
+        <c:axId val="1221776316"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -856,7 +856,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1773048964"/>
+        <c:crossAx val="627810477"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1002,11 +1002,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1538944218"/>
-        <c:axId val="1699163294"/>
+        <c:axId val="1243030851"/>
+        <c:axId val="1314643954"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1538944218"/>
+        <c:axId val="1243030851"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1058,10 +1058,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1699163294"/>
+        <c:crossAx val="1314643954"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1699163294"/>
+        <c:axId val="1314643954"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1125,7 +1125,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1538944218"/>
+        <c:crossAx val="1243030851"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1245,11 +1245,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="2055113739"/>
-        <c:axId val="670661849"/>
+        <c:axId val="1431455138"/>
+        <c:axId val="943657021"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2055113739"/>
+        <c:axId val="1431455138"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1301,10 +1301,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="670661849"/>
+        <c:crossAx val="943657021"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="670661849"/>
+        <c:axId val="943657021"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1368,7 +1368,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2055113739"/>
+        <c:crossAx val="1431455138"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1697,6 +1697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1903,23 +1904,23 @@
         <v>5000.0</v>
       </c>
       <c r="O6" s="20">
-        <v>37.53</v>
+        <v>36.8</v>
       </c>
       <c r="P6" s="20">
-        <v>37.48</v>
+        <v>36.26</v>
       </c>
       <c r="Q6" s="20">
-        <v>37.44</v>
+        <v>37.7</v>
       </c>
       <c r="R6" s="20">
-        <v>37.36</v>
+        <v>37.14</v>
       </c>
       <c r="S6" s="20">
-        <v>37.32</v>
+        <v>36.56</v>
       </c>
       <c r="T6" s="21">
         <f t="shared" ref="T6:T17" si="3">AVERAGE(O6:S6)</f>
-        <v>37.426</v>
+        <v>36.892</v>
       </c>
       <c r="U6" s="19">
         <f>T6/T6</f>
@@ -1971,31 +1972,31 @@
         <v>5000.0</v>
       </c>
       <c r="O7" s="20">
-        <v>18.61</v>
+        <v>17.59</v>
       </c>
       <c r="P7" s="20">
-        <v>17.9</v>
+        <v>18.62</v>
       </c>
       <c r="Q7" s="20">
-        <v>19.18</v>
+        <v>17.66</v>
       </c>
       <c r="R7" s="20">
-        <v>18.51</v>
+        <v>18.67</v>
       </c>
       <c r="S7" s="20">
-        <v>17.79</v>
+        <v>17.72</v>
       </c>
       <c r="T7" s="21">
         <f t="shared" si="3"/>
-        <v>18.398</v>
+        <v>18.052</v>
       </c>
       <c r="U7" s="22">
         <f>T6/T7</f>
-        <v>2.034242852</v>
+        <v>2.043651673</v>
       </c>
       <c r="V7" s="22">
         <f t="shared" si="4"/>
-        <v>1.017121426</v>
+        <v>1.021825836</v>
       </c>
     </row>
     <row r="8">
@@ -2039,31 +2040,31 @@
         <v>5000.0</v>
       </c>
       <c r="O8" s="20">
-        <v>12.86</v>
+        <v>12.64</v>
       </c>
       <c r="P8" s="20">
-        <v>11.91</v>
+        <v>11.53</v>
       </c>
       <c r="Q8" s="20">
-        <v>12.98</v>
+        <v>12.44</v>
       </c>
       <c r="R8" s="20">
-        <v>12.05</v>
+        <v>11.32</v>
       </c>
       <c r="S8" s="20">
-        <v>13.11</v>
+        <v>12.24</v>
       </c>
       <c r="T8" s="21">
         <f t="shared" si="3"/>
-        <v>12.582</v>
+        <v>12.034</v>
       </c>
       <c r="U8" s="22">
         <f>T6/T8</f>
-        <v>2.974566842</v>
+        <v>3.065647333</v>
       </c>
       <c r="V8" s="22">
         <f t="shared" si="4"/>
-        <v>0.9915222805</v>
+        <v>1.021882444</v>
       </c>
     </row>
     <row r="9">
@@ -2107,31 +2108,31 @@
         <v>5000.0</v>
       </c>
       <c r="O9" s="20">
-        <v>9.05</v>
+        <v>10.07</v>
       </c>
       <c r="P9" s="20">
-        <v>8.99</v>
+        <v>9.9</v>
       </c>
       <c r="Q9" s="20">
-        <v>9.09</v>
+        <v>9.83</v>
       </c>
       <c r="R9" s="20">
-        <v>9.04</v>
+        <v>9.66</v>
       </c>
       <c r="S9" s="20">
-        <v>8.97</v>
+        <v>9.58</v>
       </c>
       <c r="T9" s="21">
         <f t="shared" si="3"/>
-        <v>9.028</v>
+        <v>9.808</v>
       </c>
       <c r="U9" s="22">
         <f>T6/T9</f>
-        <v>4.145547187</v>
+        <v>3.76141925</v>
       </c>
       <c r="V9" s="22">
         <f t="shared" si="4"/>
-        <v>1.036386797</v>
+        <v>0.9403548124</v>
       </c>
     </row>
     <row r="10">
@@ -2175,31 +2176,31 @@
         <v>5000.0</v>
       </c>
       <c r="O10" s="20">
-        <v>7.21</v>
+        <v>7.57</v>
       </c>
       <c r="P10" s="20">
-        <v>7.3</v>
+        <v>7.55</v>
       </c>
       <c r="Q10" s="20">
-        <v>7.48</v>
+        <v>7.83</v>
       </c>
       <c r="R10" s="20">
-        <v>7.57</v>
+        <v>7.83</v>
       </c>
       <c r="S10" s="20">
-        <v>7.67</v>
+        <v>7.82</v>
       </c>
       <c r="T10" s="21">
         <f t="shared" si="3"/>
-        <v>7.446</v>
+        <v>7.72</v>
       </c>
       <c r="U10" s="22">
         <f>T6/T10</f>
-        <v>5.026322858</v>
+        <v>4.778756477</v>
       </c>
       <c r="V10" s="22">
         <f t="shared" si="4"/>
-        <v>1.005264572</v>
+        <v>0.9557512953</v>
       </c>
     </row>
     <row r="11">
@@ -2243,31 +2244,31 @@
         <v>5000.0</v>
       </c>
       <c r="O11" s="20">
-        <v>6.51</v>
+        <v>6.57</v>
       </c>
       <c r="P11" s="20">
-        <v>5.45</v>
+        <v>5.35</v>
       </c>
       <c r="Q11" s="20">
-        <v>6.31</v>
+        <v>6.13</v>
       </c>
       <c r="R11" s="20">
-        <v>7.15</v>
+        <v>6.88</v>
       </c>
       <c r="S11" s="20">
-        <v>6.09</v>
+        <v>5.83</v>
       </c>
       <c r="T11" s="21">
         <f t="shared" si="3"/>
-        <v>6.302</v>
+        <v>6.152</v>
       </c>
       <c r="U11" s="22">
         <f>T6/T11</f>
-        <v>5.938749603</v>
+        <v>5.996749025</v>
       </c>
       <c r="V11" s="22">
         <f t="shared" si="4"/>
-        <v>0.9897916006</v>
+        <v>0.9994581708</v>
       </c>
     </row>
     <row r="12">
@@ -2311,31 +2312,31 @@
         <v>5000.0</v>
       </c>
       <c r="O12" s="20">
-        <v>6.05</v>
+        <v>5.7</v>
       </c>
       <c r="P12" s="20">
-        <v>6.02</v>
+        <v>5.62</v>
       </c>
       <c r="Q12" s="20">
-        <v>5.98</v>
+        <v>6.08</v>
       </c>
       <c r="R12" s="20">
-        <v>6.06</v>
+        <v>5.96</v>
       </c>
       <c r="S12" s="20">
-        <v>6.04</v>
+        <v>5.92</v>
       </c>
       <c r="T12" s="21">
         <f t="shared" si="3"/>
-        <v>6.03</v>
+        <v>5.856</v>
       </c>
       <c r="U12" s="22">
         <f>T6/T12</f>
-        <v>6.206633499</v>
+        <v>6.299863388</v>
       </c>
       <c r="V12" s="22">
         <f t="shared" si="4"/>
-        <v>0.8866619285</v>
+        <v>0.899980484</v>
       </c>
     </row>
     <row r="13">
@@ -2379,31 +2380,31 @@
         <v>5000.0</v>
       </c>
       <c r="O13" s="20">
-        <v>5.35</v>
+        <v>5.2</v>
       </c>
       <c r="P13" s="20">
-        <v>4.75</v>
+        <v>4.46</v>
       </c>
       <c r="Q13" s="20">
-        <v>4.13</v>
+        <v>3.84</v>
       </c>
       <c r="R13" s="20">
-        <v>5.46</v>
+        <v>5.16</v>
       </c>
       <c r="S13" s="20">
-        <v>4.78</v>
+        <v>4.55</v>
       </c>
       <c r="T13" s="21">
         <f t="shared" si="3"/>
-        <v>4.894</v>
+        <v>4.642</v>
       </c>
       <c r="U13" s="22">
         <f>T6/T13</f>
-        <v>7.647323253</v>
+        <v>7.94743645</v>
       </c>
       <c r="V13" s="22">
         <f t="shared" si="4"/>
-        <v>0.9559154066</v>
+        <v>0.9934295562</v>
       </c>
     </row>
     <row r="14">
@@ -2447,31 +2448,31 @@
         <v>5000.0</v>
       </c>
       <c r="O14" s="20">
-        <v>3.57</v>
+        <v>3.32</v>
       </c>
       <c r="P14" s="20">
-        <v>4.37</v>
+        <v>4.5</v>
       </c>
       <c r="Q14" s="20">
-        <v>5.19</v>
+        <v>3.28</v>
       </c>
       <c r="R14" s="20">
-        <v>4.06</v>
+        <v>4.1</v>
       </c>
       <c r="S14" s="20">
-        <v>5.52</v>
+        <v>4.95</v>
       </c>
       <c r="T14" s="21">
         <f t="shared" si="3"/>
-        <v>4.542</v>
+        <v>4.03</v>
       </c>
       <c r="U14" s="22">
         <f>T6/T14</f>
-        <v>8.239982387</v>
+        <v>9.154342432</v>
       </c>
       <c r="V14" s="22">
         <f t="shared" si="4"/>
-        <v>0.9155535985</v>
+        <v>1.017149159</v>
       </c>
     </row>
     <row r="15">
@@ -2515,31 +2516,31 @@
         <v>5000.0</v>
       </c>
       <c r="O15" s="20">
-        <v>3.98</v>
+        <v>3.32</v>
       </c>
       <c r="P15" s="20">
-        <v>4.4</v>
+        <v>3.7</v>
       </c>
       <c r="Q15" s="20">
-        <v>2.95</v>
+        <v>4.28</v>
       </c>
       <c r="R15" s="20">
-        <v>3.59</v>
+        <v>4.63</v>
       </c>
       <c r="S15" s="20">
-        <v>4.07</v>
+        <v>2.99</v>
       </c>
       <c r="T15" s="21">
         <f t="shared" si="3"/>
-        <v>3.798</v>
+        <v>3.784</v>
       </c>
       <c r="U15" s="22">
         <f>T6/T15</f>
-        <v>9.854133755</v>
+        <v>9.749471459</v>
       </c>
       <c r="V15" s="22">
         <f t="shared" si="4"/>
-        <v>0.9854133755</v>
+        <v>0.9749471459</v>
       </c>
     </row>
     <row r="16">
@@ -2583,31 +2584,31 @@
         <v>5000.0</v>
       </c>
       <c r="O16" s="20">
-        <v>4.24</v>
+        <v>3.07</v>
       </c>
       <c r="P16" s="20">
-        <v>4.36</v>
+        <v>3.2</v>
       </c>
       <c r="Q16" s="20">
-        <v>4.52</v>
+        <v>3.26</v>
       </c>
       <c r="R16" s="20">
-        <v>3.05</v>
+        <v>3.41</v>
       </c>
       <c r="S16" s="20">
-        <v>3.21</v>
+        <v>3.49</v>
       </c>
       <c r="T16" s="21">
         <f t="shared" si="3"/>
-        <v>3.876</v>
+        <v>3.286</v>
       </c>
       <c r="U16" s="22">
         <f>T6/T16</f>
-        <v>9.655830753</v>
+        <v>11.22702374</v>
       </c>
       <c r="V16" s="22">
         <f t="shared" si="4"/>
-        <v>0.8778027958</v>
+        <v>1.020638522</v>
       </c>
     </row>
     <row r="17">
@@ -2651,31 +2652,31 @@
         <v>5000.0</v>
       </c>
       <c r="O17" s="20">
+        <v>3.74</v>
+      </c>
+      <c r="P17" s="20">
+        <v>3.97</v>
+      </c>
+      <c r="Q17" s="20">
+        <v>4.43</v>
+      </c>
+      <c r="R17" s="20">
+        <v>3.24</v>
+      </c>
+      <c r="S17" s="20">
         <v>3.41</v>
-      </c>
-      <c r="P17" s="20">
-        <v>3.79</v>
-      </c>
-      <c r="Q17" s="20">
-        <v>4.37</v>
-      </c>
-      <c r="R17" s="20">
-        <v>4.74</v>
-      </c>
-      <c r="S17" s="20">
-        <v>2.96</v>
       </c>
       <c r="T17" s="21">
         <f t="shared" si="3"/>
-        <v>3.854</v>
+        <v>3.758</v>
       </c>
       <c r="U17" s="22">
         <f>T6/T17</f>
-        <v>9.710949663</v>
+        <v>9.816923896</v>
       </c>
       <c r="V17" s="22">
         <f t="shared" si="4"/>
-        <v>0.8092458052</v>
+        <v>0.8180769913</v>
       </c>
     </row>
     <row r="18">
@@ -2823,23 +2824,23 @@
         <v>5000.0</v>
       </c>
       <c r="O21" s="18">
-        <v>36.92</v>
+        <v>36.87</v>
       </c>
       <c r="P21" s="18">
-        <v>36.87</v>
+        <v>36.28</v>
       </c>
       <c r="Q21" s="18">
-        <v>36.82</v>
+        <v>37.72</v>
       </c>
       <c r="R21" s="18">
-        <v>36.73</v>
+        <v>37.17</v>
       </c>
       <c r="S21" s="18">
-        <v>36.64</v>
+        <v>36.63</v>
       </c>
       <c r="T21" s="19">
         <f t="shared" ref="T21:T32" si="6">AVERAGE(O21:S21)</f>
-        <v>36.796</v>
+        <v>36.934</v>
       </c>
       <c r="U21" s="19">
         <f>T21/T21</f>
@@ -2885,27 +2886,27 @@
         <v>7000.0</v>
       </c>
       <c r="O22" s="18">
-        <v>35.8</v>
+        <v>35.32</v>
       </c>
       <c r="P22" s="18">
-        <v>36.96</v>
+        <v>36.0</v>
       </c>
       <c r="Q22" s="18">
-        <v>36.16</v>
+        <v>36.68</v>
       </c>
       <c r="R22" s="18">
-        <v>37.32</v>
+        <v>35.38</v>
       </c>
       <c r="S22" s="18">
-        <v>36.52</v>
+        <v>36.08</v>
       </c>
       <c r="T22" s="19">
         <f t="shared" si="6"/>
-        <v>36.552</v>
+        <v>35.892</v>
       </c>
       <c r="U22" s="22">
         <f>T21/T22</f>
-        <v>1.006675421</v>
+        <v>1.029031539</v>
       </c>
       <c r="V22" s="19"/>
     </row>
@@ -2947,27 +2948,27 @@
         <v>8550.0</v>
       </c>
       <c r="O23" s="18">
-        <v>35.49</v>
+        <v>36.59</v>
       </c>
       <c r="P23" s="18">
-        <v>36.47</v>
+        <v>35.09</v>
       </c>
       <c r="Q23" s="18">
-        <v>35.44</v>
+        <v>35.6</v>
       </c>
       <c r="R23" s="18">
-        <v>36.4</v>
+        <v>36.11</v>
       </c>
       <c r="S23" s="18">
-        <v>37.37</v>
+        <v>37.6</v>
       </c>
       <c r="T23" s="19">
         <f t="shared" si="6"/>
-        <v>36.234</v>
+        <v>36.198</v>
       </c>
       <c r="U23" s="22">
         <f>T21/T23</f>
-        <v>1.015510294</v>
+        <v>1.020332615</v>
       </c>
       <c r="V23" s="19"/>
     </row>
@@ -3009,27 +3010,27 @@
         <v>9950.0</v>
       </c>
       <c r="O24" s="18">
-        <v>36.92</v>
+        <v>35.68</v>
       </c>
       <c r="P24" s="18">
-        <v>37.0</v>
+        <v>36.74</v>
       </c>
       <c r="Q24" s="18">
-        <v>36.53</v>
+        <v>35.82</v>
       </c>
       <c r="R24" s="18">
-        <v>36.05</v>
+        <v>37.99</v>
       </c>
       <c r="S24" s="18">
-        <v>37.54</v>
+        <v>37.76</v>
       </c>
       <c r="T24" s="19">
         <f t="shared" si="6"/>
-        <v>36.808</v>
+        <v>36.798</v>
       </c>
       <c r="U24" s="22">
         <f>T21/T24</f>
-        <v>0.9996739839</v>
+        <v>1.003695853</v>
       </c>
       <c r="V24" s="19"/>
     </row>
@@ -3071,27 +3072,27 @@
         <v>11100.0</v>
       </c>
       <c r="O25" s="18">
-        <v>36.9</v>
+        <v>36.66</v>
       </c>
       <c r="P25" s="18">
-        <v>36.27</v>
+        <v>35.57</v>
       </c>
       <c r="Q25" s="18">
-        <v>42.92</v>
+        <v>36.49</v>
       </c>
       <c r="R25" s="18">
-        <v>36.27</v>
+        <v>35.42</v>
       </c>
       <c r="S25" s="18">
-        <v>37.64</v>
+        <v>36.31</v>
       </c>
       <c r="T25" s="19">
         <f t="shared" si="6"/>
-        <v>38</v>
+        <v>36.09</v>
       </c>
       <c r="U25" s="22">
         <f>T21/T25</f>
-        <v>0.9683157895</v>
+        <v>1.023385979</v>
       </c>
       <c r="V25" s="19"/>
     </row>
@@ -3133,27 +3134,27 @@
         <v>12150.0</v>
       </c>
       <c r="O26" s="18">
-        <v>36.94</v>
+        <v>37.17</v>
       </c>
       <c r="P26" s="18">
-        <v>36.29</v>
+        <v>36.02</v>
       </c>
       <c r="Q26" s="18">
-        <v>37.72</v>
+        <v>42.06</v>
       </c>
       <c r="R26" s="18">
-        <v>37.83</v>
+        <v>38.38</v>
       </c>
       <c r="S26" s="18">
-        <v>37.14</v>
+        <v>40.92</v>
       </c>
       <c r="T26" s="19">
         <f t="shared" si="6"/>
-        <v>37.184</v>
+        <v>38.91</v>
       </c>
       <c r="U26" s="22">
         <f>T21/T26</f>
-        <v>0.9895654045</v>
+        <v>0.9492161398</v>
       </c>
       <c r="V26" s="19"/>
     </row>
@@ -3195,27 +3196,27 @@
         <v>13150.0</v>
       </c>
       <c r="O27" s="18">
-        <v>41.92</v>
+        <v>35.93</v>
       </c>
       <c r="P27" s="18">
-        <v>37.4</v>
+        <v>36.92</v>
       </c>
       <c r="Q27" s="18">
-        <v>36.87</v>
+        <v>35.93</v>
       </c>
       <c r="R27" s="18">
-        <v>37.81</v>
+        <v>36.92</v>
       </c>
       <c r="S27" s="18">
-        <v>37.27</v>
+        <v>35.96</v>
       </c>
       <c r="T27" s="19">
         <f t="shared" si="6"/>
-        <v>38.254</v>
+        <v>36.332</v>
       </c>
       <c r="U27" s="22">
         <f>T21/T27</f>
-        <v>0.9618863387</v>
+        <v>1.016569415</v>
       </c>
       <c r="V27" s="19"/>
     </row>
@@ -3257,27 +3258,27 @@
         <v>14000.0</v>
       </c>
       <c r="O28" s="18">
-        <v>36.48</v>
+        <v>41.85</v>
       </c>
       <c r="P28" s="18">
-        <v>35.67</v>
+        <v>36.6</v>
       </c>
       <c r="Q28" s="18">
-        <v>36.85</v>
+        <v>39.02</v>
       </c>
       <c r="R28" s="18">
-        <v>36.06</v>
+        <v>35.76</v>
       </c>
       <c r="S28" s="18">
-        <v>37.3</v>
+        <v>36.52</v>
       </c>
       <c r="T28" s="19">
         <f t="shared" si="6"/>
-        <v>36.472</v>
+        <v>37.95</v>
       </c>
       <c r="U28" s="22">
         <f>T21/T28</f>
-        <v>1.008883527</v>
+        <v>0.9732279315</v>
       </c>
       <c r="V28" s="19"/>
     </row>
@@ -3319,27 +3320,27 @@
         <v>14850.0</v>
       </c>
       <c r="O29" s="18">
-        <v>37.65</v>
+        <v>35.31</v>
       </c>
       <c r="P29" s="18">
-        <v>36.89</v>
+        <v>36.06</v>
       </c>
       <c r="Q29" s="18">
-        <v>36.19</v>
+        <v>36.85</v>
       </c>
       <c r="R29" s="18">
-        <v>37.41</v>
+        <v>37.07</v>
       </c>
       <c r="S29" s="18">
-        <v>36.67</v>
+        <v>35.84</v>
       </c>
       <c r="T29" s="19">
         <f t="shared" si="6"/>
-        <v>36.962</v>
+        <v>36.226</v>
       </c>
       <c r="U29" s="22">
         <f>T21/T29</f>
-        <v>0.995508901</v>
+        <v>1.019543974</v>
       </c>
       <c r="V29" s="19"/>
     </row>
@@ -3381,27 +3382,27 @@
         <v>15750.0</v>
       </c>
       <c r="O30" s="18">
-        <v>36.36</v>
+        <v>37.07</v>
       </c>
       <c r="P30" s="18">
-        <v>36.13</v>
+        <v>36.72</v>
       </c>
       <c r="Q30" s="18">
-        <v>37.82</v>
+        <v>35.96</v>
       </c>
       <c r="R30" s="18">
-        <v>42.76</v>
+        <v>37.17</v>
       </c>
       <c r="S30" s="18">
-        <v>36.42</v>
+        <v>36.46</v>
       </c>
       <c r="T30" s="19">
         <f t="shared" si="6"/>
-        <v>37.898</v>
+        <v>36.676</v>
       </c>
       <c r="U30" s="22">
         <f>T21/T30</f>
-        <v>0.9709219484</v>
+        <v>1.007034573</v>
       </c>
       <c r="V30" s="19"/>
     </row>
@@ -3443,27 +3444,27 @@
         <v>16400.0</v>
       </c>
       <c r="O31" s="18">
-        <v>35.84</v>
+        <v>35.35</v>
       </c>
       <c r="P31" s="18">
-        <v>37.27</v>
+        <v>36.38</v>
       </c>
       <c r="Q31" s="18">
-        <v>37.16</v>
+        <v>36.9</v>
       </c>
       <c r="R31" s="18">
-        <v>36.5</v>
+        <v>37.44</v>
       </c>
       <c r="S31" s="18">
-        <v>36.4</v>
+        <v>36.65</v>
       </c>
       <c r="T31" s="19">
         <f t="shared" si="6"/>
-        <v>36.634</v>
+        <v>36.544</v>
       </c>
       <c r="U31" s="22">
         <f>T21/T31</f>
-        <v>1.004422122</v>
+        <v>1.010672067</v>
       </c>
       <c r="V31" s="19"/>
     </row>
@@ -3505,27 +3506,27 @@
         <v>17250.0</v>
       </c>
       <c r="O32" s="18">
-        <v>40.79</v>
+        <v>40.11</v>
       </c>
       <c r="P32" s="18">
-        <v>40.29</v>
+        <v>41.13</v>
       </c>
       <c r="Q32" s="18">
-        <v>41.74</v>
+        <v>40.12</v>
       </c>
       <c r="R32" s="18">
-        <v>42.1</v>
+        <v>41.17</v>
       </c>
       <c r="S32" s="18">
-        <v>41.67</v>
+        <v>40.42</v>
       </c>
       <c r="T32" s="19">
         <f t="shared" si="6"/>
-        <v>41.318</v>
+        <v>40.59</v>
       </c>
       <c r="U32" s="22">
         <f>T21/T32</f>
-        <v>0.8905561741</v>
+        <v>0.9099285538</v>
       </c>
       <c r="V32" s="19"/>
     </row>
@@ -3542,6 +3543,9 @@
     <mergeCell ref="M18:V18"/>
     <mergeCell ref="M19:V19"/>
   </mergeCells>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>